<commit_message>
Finished PT_Plan v1.0 and system test related documents
</commit_message>
<xml_diff>
--- a/test-doc/功能测试用例_G06_v1.0.xlsx
+++ b/test-doc/功能测试用例_G06_v1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9420" tabRatio="612" activeTab="5"/>
+    <workbookView windowWidth="23040" windowHeight="9420" tabRatio="612"/>
   </bookViews>
   <sheets>
     <sheet name="变更记录" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="287">
   <si>
     <t>变更历史记录</t>
   </si>
@@ -145,6 +145,9 @@
     <t>是</t>
   </si>
   <si>
+    <t>通过</t>
+  </si>
+  <si>
     <t>用户名为空</t>
   </si>
   <si>
@@ -155,6 +158,9 @@
     <t>1.登录失败，显示提示</t>
   </si>
   <si>
+    <t>否</t>
+  </si>
+  <si>
     <t>用户名错误</t>
   </si>
   <si>
@@ -236,6 +242,9 @@
   </si>
   <si>
     <t>1.列出所有ID和输入匹配的项目</t>
+  </si>
+  <si>
+    <t>删除用例</t>
   </si>
   <si>
     <t>正常查询(按项目经理)</t>
@@ -1126,14 +1135,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1168,6 +1185,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="等线"/>
@@ -1182,24 +1207,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1229,8 +1238,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1254,15 +1264,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1271,6 +1273,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1291,7 +1300,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1315,43 +1444,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1363,79 +1468,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1447,31 +1480,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1810,6 +1819,21 @@
       </top>
       <bottom style="thick">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1838,15 +1862,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1864,11 +1879,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1897,69 +1910,65 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1968,94 +1977,94 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2595,8 +2604,8 @@
   <sheetPr/>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelCol="3"/>
@@ -2819,7 +2828,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -2954,7 +2963,9 @@
       <c r="G8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="16"/>
+      <c r="H8" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="I8" s="7"/>
     </row>
     <row r="9" ht="31.2" spans="1:9">
@@ -2965,21 +2976,23 @@
         <v>35</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>37</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="I9" s="7"/>
     </row>
     <row r="10" ht="31.2" spans="1:9">
@@ -2990,21 +3003,23 @@
         <v>35</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>37</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="16"/>
+      <c r="H10" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="I10" s="7"/>
     </row>
     <row r="11" ht="46.8" spans="1:9">
@@ -3015,21 +3030,23 @@
         <v>35</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>37</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="16"/>
+      <c r="H11" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="I11" s="7"/>
     </row>
     <row r="12" ht="31.2" spans="1:9">
@@ -3040,21 +3057,23 @@
         <v>35</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>37</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="I12" s="7"/>
     </row>
     <row r="13" ht="31.2" spans="1:9">
@@ -3065,21 +3084,23 @@
         <v>35</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>37</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="16"/>
+      <c r="H13" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="I13" s="7"/>
     </row>
     <row r="14" s="9" customFormat="1" ht="46.8" spans="1:9">
@@ -3090,21 +3111,23 @@
         <v>35</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>37</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="16"/>
+      <c r="H14" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="I14" s="7"/>
     </row>
     <row r="15" s="9" customFormat="1" ht="31.2" spans="1:9">
@@ -3115,21 +3138,23 @@
         <v>35</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>37</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="I15" s="7"/>
     </row>
     <row r="16" ht="31.2" spans="1:9">
@@ -3140,21 +3165,23 @@
         <v>35</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>37</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="16"/>
+      <c r="H16" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="I16" s="7"/>
     </row>
     <row r="17" ht="47.55" spans="1:9">
@@ -3165,21 +3192,23 @@
         <v>35</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>37</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G17" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="21"/>
+      <c r="H17" s="21" t="s">
+        <v>41</v>
+      </c>
       <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:8">
@@ -3218,7 +3247,7 @@
   <dimension ref="A1:I156"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -3343,24 +3372,26 @@
         <v>1</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="16"/>
+      <c r="H8" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="I8" s="49"/>
     </row>
     <row r="9" ht="46.8" spans="1:9">
@@ -3368,24 +3399,26 @@
         <v>2</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="16"/>
+      <c r="H9" s="16" t="s">
+        <v>70</v>
+      </c>
       <c r="I9" s="49"/>
     </row>
     <row r="10" ht="46.8" spans="1:9">
@@ -3393,24 +3426,26 @@
         <v>3</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="16"/>
+      <c r="H10" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="I10" s="49"/>
     </row>
     <row r="11" s="35" customFormat="1" ht="46.8" spans="1:9">
@@ -3418,24 +3453,26 @@
         <v>4</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="16"/>
+      <c r="H11" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="I11" s="49"/>
     </row>
     <row r="12" ht="31.2" spans="1:9">
@@ -3443,24 +3480,26 @@
         <v>5</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="16"/>
+      <c r="H12" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="I12" s="49"/>
     </row>
     <row r="13" ht="46.8" spans="1:9">
@@ -3468,24 +3507,26 @@
         <v>6</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="16"/>
+      <c r="H13" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="I13" s="49"/>
     </row>
     <row r="14" ht="46.8" spans="1:9">
@@ -3493,24 +3534,26 @@
         <v>7</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="16"/>
+      <c r="H14" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="I14" s="49"/>
     </row>
     <row r="15" ht="31.95" spans="1:9">
@@ -3518,24 +3561,26 @@
         <v>8</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="21"/>
+      <c r="H15" s="21" t="s">
+        <v>41</v>
+      </c>
       <c r="I15" s="49"/>
     </row>
     <row r="16" spans="1:8">
@@ -4961,7 +5006,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.2" defaultRowHeight="15.6" outlineLevelCol="7"/>
@@ -5086,21 +5131,23 @@
         <v>35</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" ht="31.2" spans="1:8">
       <c r="A9" s="29">
@@ -5110,141 +5157,153 @@
         <v>35</v>
       </c>
       <c r="C9" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>86</v>
-      </c>
       <c r="E9" s="9" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" ht="62.4" spans="1:8">
       <c r="A10" s="29">
         <v>3</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" ht="62.4" spans="1:8">
       <c r="A11" s="29">
         <v>4</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C11" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>93</v>
-      </c>
       <c r="E11" s="9" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" ht="78" spans="1:8">
       <c r="A12" s="29">
         <v>5</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="13" ht="62.4" spans="1:8">
       <c r="A13" s="29">
         <v>6</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="14" ht="94.35" spans="1:8">
       <c r="A14" s="33">
         <v>7</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="32"/>
+        <v>45</v>
+      </c>
+      <c r="H14" s="32" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -5270,8 +5329,8 @@
   <sheetPr/>
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.2" defaultRowHeight="15.6" outlineLevelCol="7"/>
@@ -5393,1536 +5452,1664 @@
         <v>1</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="62.4" spans="1:8">
       <c r="A9" s="29">
         <v>2</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D9" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>113</v>
-      </c>
       <c r="F9" s="9" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" s="1" customFormat="1" ht="109.2" spans="1:8">
       <c r="A10" s="29">
         <v>3</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" s="1" customFormat="1" ht="109.2" spans="1:8">
       <c r="A11" s="29">
         <v>4</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D11" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>119</v>
-      </c>
       <c r="F11" s="9" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" s="1" customFormat="1" ht="93.6" spans="1:8">
       <c r="A12" s="29">
         <v>5</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="13" s="1" customFormat="1" ht="93.6" spans="1:8">
       <c r="A13" s="29">
         <v>6</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="14" s="1" customFormat="1" ht="93.6" spans="1:8">
       <c r="A14" s="29">
         <v>7</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="15" s="1" customFormat="1" ht="93.6" spans="1:8">
       <c r="A15" s="29">
         <v>8</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="16" s="1" customFormat="1" ht="93.6" spans="1:8">
       <c r="A16" s="29">
         <v>9</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="17" s="1" customFormat="1" ht="109.2" spans="1:8">
       <c r="A17" s="29">
         <v>10</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="18" s="1" customFormat="1" ht="93.6" spans="1:8">
       <c r="A18" s="29">
         <v>11</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H18" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="19" ht="109.2" spans="1:8">
       <c r="A19" s="29">
         <v>12</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H19" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="20" ht="93.6" spans="1:8">
       <c r="A20" s="29">
         <v>13</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="21" ht="109.2" spans="1:8">
       <c r="A21" s="29">
         <v>14</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H21" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H21" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="22" ht="78" spans="1:8">
       <c r="A22" s="29">
         <v>15</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H22" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H22" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="23" ht="93.6" spans="1:8">
       <c r="A23" s="29">
         <v>16</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H23" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H23" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="24" ht="62.4" spans="1:8">
       <c r="A24" s="29">
         <v>17</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H24" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H24" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="25" s="1" customFormat="1" ht="62.4" spans="1:8">
       <c r="A25" s="29">
         <v>18</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H25" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H25" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="26" s="1" customFormat="1" ht="62.4" spans="1:8">
       <c r="A26" s="29">
         <v>19</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H26" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H26" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="27" s="1" customFormat="1" ht="62.4" spans="1:8">
       <c r="A27" s="29">
         <v>20</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H27" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H27" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="28" s="1" customFormat="1" ht="62.4" spans="1:8">
       <c r="A28" s="29">
         <v>21</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E28" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="F28" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="F28" s="12" t="s">
-        <v>167</v>
-      </c>
       <c r="G28" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H28" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H28" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="29" s="1" customFormat="1" ht="62.4" spans="1:8">
       <c r="A29" s="29">
         <v>22</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E29" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="F29" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="F29" s="12" t="s">
-        <v>167</v>
-      </c>
       <c r="G29" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H29" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H29" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="30" ht="78" spans="1:8">
       <c r="A30" s="29">
         <v>23</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H30" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H30" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="31" s="1" customFormat="1" ht="78" spans="1:8">
       <c r="A31" s="29">
         <v>24</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D31" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="E31" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="E31" s="12" t="s">
-        <v>174</v>
-      </c>
       <c r="F31" s="12" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H31" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H31" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="32" s="1" customFormat="1" ht="78" spans="1:8">
       <c r="A32" s="29">
         <v>25</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H32" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H32" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="33" s="1" customFormat="1" ht="78" spans="1:8">
       <c r="A33" s="29">
         <v>26</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C33" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="D33" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="D33" s="12" t="s">
-        <v>177</v>
-      </c>
       <c r="E33" s="12" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H33" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H33" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="34" s="1" customFormat="1" ht="78" spans="1:8">
       <c r="A34" s="29">
         <v>27</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H34" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H34" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="35" s="1" customFormat="1" ht="78" spans="1:8">
       <c r="A35" s="29">
         <v>28</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H35" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H35" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="36" ht="78" spans="1:8">
       <c r="A36" s="29">
         <v>29</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H36" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H36" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="37" s="1" customFormat="1" ht="78" spans="1:8">
       <c r="A37" s="29">
         <v>30</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C37" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D37" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="D37" s="12" t="s">
-        <v>185</v>
-      </c>
       <c r="E37" s="12" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H37" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H37" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="38" s="1" customFormat="1" ht="78" spans="1:8">
       <c r="A38" s="29">
         <v>31</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H38" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H38" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="39" s="1" customFormat="1" ht="78" spans="1:8">
       <c r="A39" s="29">
         <v>32</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C39" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="F39" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="D39" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>190</v>
-      </c>
       <c r="G39" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H39" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H39" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="40" s="1" customFormat="1" ht="78" spans="1:8">
       <c r="A40" s="29">
         <v>33</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H40" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H40" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="41" s="1" customFormat="1" ht="78" spans="1:8">
       <c r="A41" s="29">
         <v>34</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H41" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H41" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="42" s="1" customFormat="1" ht="78" spans="1:8">
       <c r="A42" s="29">
         <v>35</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C42" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="F42" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="D42" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F42" s="12" t="s">
-        <v>196</v>
-      </c>
       <c r="G42" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H42" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H42" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="43" s="1" customFormat="1" ht="78" spans="1:8">
       <c r="A43" s="29">
         <v>36</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H43" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H43" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="44" ht="93.6" spans="1:8">
       <c r="A44" s="29">
         <v>37</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H44" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H44" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="45" s="1" customFormat="1" ht="93.6" spans="1:8">
       <c r="A45" s="29">
         <v>38</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D45" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="E45" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="E45" s="12" t="s">
-        <v>203</v>
-      </c>
       <c r="F45" s="12" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H45" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H45" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="46" s="1" customFormat="1" ht="93.6" spans="1:8">
       <c r="A46" s="29">
         <v>39</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H46" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H46" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="47" s="1" customFormat="1" ht="93.6" spans="1:8">
       <c r="A47" s="29">
         <v>40</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C47" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F47" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="D47" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="F47" s="12" t="s">
-        <v>207</v>
-      </c>
       <c r="G47" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H47" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H47" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="48" s="1" customFormat="1" ht="93.6" spans="1:8">
       <c r="A48" s="29">
         <v>41</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H48" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H48" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="49" s="1" customFormat="1" ht="93.6" spans="1:8">
       <c r="A49" s="29">
         <v>42</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H49" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H49" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="50" s="1" customFormat="1" ht="93.6" spans="1:8">
       <c r="A50" s="29">
         <v>43</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C50" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="F50" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="D50" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="F50" s="12" t="s">
-        <v>214</v>
-      </c>
       <c r="G50" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H50" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H50" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="51" s="1" customFormat="1" ht="93.6" spans="1:8">
       <c r="A51" s="29">
         <v>44</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H51" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H51" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="52" ht="93.6" spans="1:8">
       <c r="A52" s="29">
         <v>45</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="F52" s="12" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H52" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H52" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="53" ht="62.4" spans="1:8">
       <c r="A53" s="29">
         <v>46</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="F53" s="12" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H53" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H53" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="54" ht="62.4" spans="1:8">
       <c r="A54" s="29">
         <v>47</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H54" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H54" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="55" ht="124.8" spans="1:8">
       <c r="A55" s="29">
         <v>48</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H55" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H55" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="56" s="1" customFormat="1" ht="93.6" spans="1:8">
       <c r="A56" s="29">
         <v>49</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H56" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H56" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="57" s="1" customFormat="1" ht="62.4" spans="1:8">
       <c r="A57" s="29">
         <v>50</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H57" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H57" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="58" s="1" customFormat="1" ht="62.4" spans="1:8">
       <c r="A58" s="29">
         <v>51</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C58" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="F58" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="D58" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="E58" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="F58" s="12" t="s">
-        <v>236</v>
-      </c>
       <c r="G58" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H58" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H58" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="59" s="1" customFormat="1" ht="124.8" spans="1:8">
       <c r="A59" s="29">
         <v>52</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="F59" s="12" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H59" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H59" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="60" ht="93.6" spans="1:8">
       <c r="A60" s="29">
         <v>53</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H60" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H60" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="61" ht="124.8" spans="1:8">
       <c r="A61" s="29">
         <v>54</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="F61" s="12" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H61" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H61" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="62" ht="124.8" spans="1:8">
       <c r="A62" s="29">
         <v>55</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D62" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="E62" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="E62" s="12" t="s">
-        <v>249</v>
-      </c>
       <c r="F62" s="12" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H62" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H62" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="63" ht="124.8" spans="1:8">
       <c r="A63" s="29">
         <v>56</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="F63" s="12" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H63" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H63" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="64" ht="124.8" spans="1:8">
       <c r="A64" s="29">
         <v>57</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C64" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="D64" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="D64" s="12" t="s">
-        <v>255</v>
-      </c>
       <c r="E64" s="12" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="F64" s="12" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H64" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H64" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="65" ht="93.6" spans="1:8">
       <c r="A65" s="29">
         <v>58</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="F65" s="12" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H65" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H65" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="66" ht="109.2" spans="1:8">
       <c r="A66" s="29">
         <v>59</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C66" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="D66" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="D66" s="12" t="s">
-        <v>262</v>
-      </c>
       <c r="E66" s="12" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F66" s="12" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H66" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H66" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="67" ht="62.4" spans="1:8">
       <c r="A67" s="29">
         <v>60</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C67" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="E67" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="F67" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="D67" s="12" t="s">
-        <v>262</v>
-      </c>
-      <c r="E67" s="12" t="s">
-        <v>268</v>
-      </c>
-      <c r="F67" s="12" t="s">
-        <v>264</v>
-      </c>
       <c r="G67" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H67" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H67" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="68" ht="78" spans="1:8">
       <c r="A68" s="29">
         <v>61</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="F68" s="12" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="G68" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H68" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H68" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="69" ht="78" spans="1:8">
       <c r="A69" s="29">
         <v>62</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E69" s="12" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="F69" s="12" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H69" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H69" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="70" ht="78" spans="1:8">
       <c r="A70" s="29">
         <v>63</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="F70" s="12" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H70" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="H70" s="30" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="71" ht="78.75" spans="1:8">
       <c r="A71" s="31">
         <v>64</v>
       </c>
       <c r="B71" s="20" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="D71" s="19" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="E71" s="19" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="F71" s="19" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="G71" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="H71" s="32"/>
+        <v>45</v>
+      </c>
+      <c r="H71" s="32" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>